<commit_message>
Antes concertar bug cartao janeiro
</commit_message>
<xml_diff>
--- a/Arquivos/Casamento.xlsx
+++ b/Arquivos/Casamento.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\Xampp\htdocs\Testes\Controle_Financeiro\Arquivos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Controle_Financeiro\Arquivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6587AD1E-393A-4238-871B-8BE12224617E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5EC4768-2094-43FA-AF82-84826318720B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0F9FFE06-2AA6-4487-9298-8CC079301120}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0F9FFE06-2AA6-4487-9298-8CC079301120}"/>
   </bookViews>
   <sheets>
     <sheet name="Geral" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="74">
   <si>
     <t>Tipo</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Fechado</t>
   </si>
   <si>
-    <t>Pesquisando</t>
-  </si>
-  <si>
     <t>Naldinho &amp; Edileuza</t>
   </si>
   <si>
@@ -147,9 +144,6 @@
     <t>Pulseira - Madrinhas</t>
   </si>
   <si>
-    <t>Dj D-30</t>
-  </si>
-  <si>
     <t>Pagamentos Até Data do Casamento</t>
   </si>
   <si>
@@ -210,10 +204,58 @@
     <t>Bar</t>
   </si>
   <si>
-    <t>MK Drinks</t>
-  </si>
-  <si>
     <t>Arts Visual</t>
+  </si>
+  <si>
+    <t>Dj Pedro Hiago</t>
+  </si>
+  <si>
+    <t>Convite (Cerveja - Padrinhos)</t>
+  </si>
+  <si>
+    <t>Convite (Copos - Pajem)</t>
+  </si>
+  <si>
+    <t>Convite (Copos - Doces - Pajem)</t>
+  </si>
+  <si>
+    <t>Roupa (Sapato Noivo)</t>
+  </si>
+  <si>
+    <t>Roupa (Sapato Noiva)</t>
+  </si>
+  <si>
+    <t>Dj D-5</t>
+  </si>
+  <si>
+    <t>Decoração - Entrada</t>
+  </si>
+  <si>
+    <t>Contato</t>
+  </si>
+  <si>
+    <t>(11) 98624-8584</t>
+  </si>
+  <si>
+    <t>(11) 94000-0503</t>
+  </si>
+  <si>
+    <t>(11) 94855-9556</t>
+  </si>
+  <si>
+    <t>(11) 97324-7775</t>
+  </si>
+  <si>
+    <t>(11) 2671-8800</t>
+  </si>
+  <si>
+    <t>TM Drinks</t>
+  </si>
+  <si>
+    <t>(11) 95885-4014</t>
+  </si>
+  <si>
+    <t>(11) 99497-4476</t>
   </si>
 </sst>
 </file>
@@ -224,7 +266,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -283,6 +325,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -310,22 +359,11 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="6"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="6"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -389,73 +427,71 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
+  <dxfs count="28">
     <dxf>
       <font>
         <color theme="0" tint="-0.24994659260841701"/>
@@ -912,49 +948,50 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{868B1771-212D-4176-97CE-969EE0F196FC}" name="Tabela1" displayName="Tabela1" ref="B2:J18" totalsRowShown="0" headerRowDxfId="29">
-  <autoFilter ref="B2:J18" xr:uid="{FE260ABD-8A2E-4709-B182-93DCF823B24F}"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{868B1771-212D-4176-97CE-969EE0F196FC}" name="Tabela1" displayName="Tabela1" ref="B2:K18" totalsRowShown="0" headerRowDxfId="27">
+  <autoFilter ref="B2:K18" xr:uid="{FE260ABD-8A2E-4709-B182-93DCF823B24F}"/>
+  <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{DD98093E-2F29-447D-BE5D-B60B73441147}" name="Tipo"/>
     <tableColumn id="10" xr3:uid="{AE42F758-EA3C-4875-B1F1-FE996BF6DE4F}" name="STATUS"/>
     <tableColumn id="2" xr3:uid="{D1B71966-EE75-44AD-8382-52E0A5ED8B60}" name="Empresa"/>
-    <tableColumn id="4" xr3:uid="{4FDC9052-72C2-4AB1-A46E-E4D7917F4F18}" name="André &amp; Fernanda" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{4B64D155-8141-4569-83D2-98EEA05248FB}" name="Vastenir &amp; Valmir" dataDxfId="27"/>
-    <tableColumn id="11" xr3:uid="{B1FC6398-1FA3-4EF1-9401-C8102EFCC5DD}" name="Naldinho &amp; Edileuza" dataDxfId="26"/>
-    <tableColumn id="6" xr3:uid="{4C2C1B08-27CF-40C8-90E1-AB7A5D180552}" name="Paula" dataDxfId="25"/>
-    <tableColumn id="7" xr3:uid="{9D781EDA-A719-4E10-9EC0-232BA236F1F7}" name="Presentes Casamento" dataDxfId="24"/>
-    <tableColumn id="8" xr3:uid="{9D4CBF35-D638-4316-9EA7-3C02514913C3}" name="Total" dataDxfId="23"/>
+    <tableColumn id="9" xr3:uid="{B73AA396-50ED-4C8E-ADC6-C9AD2EE8052F}" name="Contato"/>
+    <tableColumn id="4" xr3:uid="{4FDC9052-72C2-4AB1-A46E-E4D7917F4F18}" name="André &amp; Fernanda" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{4B64D155-8141-4569-83D2-98EEA05248FB}" name="Vastenir &amp; Valmir" dataDxfId="25"/>
+    <tableColumn id="11" xr3:uid="{B1FC6398-1FA3-4EF1-9401-C8102EFCC5DD}" name="Naldinho &amp; Edileuza" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{4C2C1B08-27CF-40C8-90E1-AB7A5D180552}" name="Paula" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{9D781EDA-A719-4E10-9EC0-232BA236F1F7}" name="Presentes Casamento" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{9D4CBF35-D638-4316-9EA7-3C02514913C3}" name="Total" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{34CD3302-267D-4AD2-B1A7-AFD15DDDEA63}" name="Tabela2" displayName="Tabela2" ref="B3:E23" totalsRowShown="0" headerRowDxfId="22" tableBorderDxfId="21">
-  <autoFilter ref="B3:E23" xr:uid="{E8401F74-9508-4443-996B-86771A12CDEF}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:E23">
-    <sortCondition ref="C3:C23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{34CD3302-267D-4AD2-B1A7-AFD15DDDEA63}" name="Tabela2" displayName="Tabela2" ref="B3:E27" totalsRowShown="0" headerRowDxfId="20" tableBorderDxfId="19">
+  <autoFilter ref="B3:E27" xr:uid="{E8401F74-9508-4443-996B-86771A12CDEF}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:E27">
+    <sortCondition ref="C3:C27"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{24D73CFF-7943-4B97-8407-DF242EC852D3}" name="Tipo" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{F303E85E-63E6-4DA2-8027-4671A362C5AF}" name="Data Pagamento(s)" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{96713C74-33D5-445F-8D71-C0AD9BA5B01D}" name="Pendente" dataDxfId="18" dataCellStyle="Moeda"/>
-    <tableColumn id="4" xr3:uid="{A272F446-7463-4570-8AB7-38C0AF883346}" name="Pago" dataDxfId="17" dataCellStyle="Moeda"/>
+    <tableColumn id="1" xr3:uid="{24D73CFF-7943-4B97-8407-DF242EC852D3}" name="Tipo" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{F303E85E-63E6-4DA2-8027-4671A362C5AF}" name="Data Pagamento(s)" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{96713C74-33D5-445F-8D71-C0AD9BA5B01D}" name="Pendente" dataDxfId="16" dataCellStyle="Moeda"/>
+    <tableColumn id="4" xr3:uid="{A272F446-7463-4570-8AB7-38C0AF883346}" name="Pago" dataDxfId="15" dataCellStyle="Moeda"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7E5A4C28-D983-4FBC-AD38-5B23712728A7}" name="Tabela3" displayName="Tabela3" ref="B28:E31" totalsRowCount="1" headerRowDxfId="16">
-  <autoFilter ref="B28:E30" xr:uid="{6A26D391-F521-4673-8CDA-D2A603414B10}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7E5A4C28-D983-4FBC-AD38-5B23712728A7}" name="Tabela3" displayName="Tabela3" ref="B32:E35" totalsRowCount="1" headerRowDxfId="14">
+  <autoFilter ref="B32:E34" xr:uid="{6A26D391-F521-4673-8CDA-D2A603414B10}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{2B0EC398-0A62-4753-B4C0-363D083E0FC3}" name="Tipo"/>
-    <tableColumn id="2" xr3:uid="{2413DB78-B117-44A7-A3A2-FC9A644BBA0F}" name="Data Pagamento(s)" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{0F539585-E6A9-41EF-B3CB-20B7C4ABCCA0}" name="Pendente" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="12" dataCellStyle="Moeda" totalsRowCellStyle="Moeda">
-      <totalsRowFormula>SUM(D29:D30)</totalsRowFormula>
+    <tableColumn id="2" xr3:uid="{2413DB78-B117-44A7-A3A2-FC9A644BBA0F}" name="Data Pagamento(s)" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{0F539585-E6A9-41EF-B3CB-20B7C4ABCCA0}" name="Pendente" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="10" dataCellStyle="Moeda" totalsRowCellStyle="Moeda">
+      <totalsRowFormula>SUM(D33:D34)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{4BC49145-FAE4-4E4E-ACE7-0BAF09922CFD}" name="Pago" dataDxfId="11" totalsRowDxfId="10" dataCellStyle="Moeda" totalsRowCellStyle="Moeda"/>
+    <tableColumn id="4" xr3:uid="{4BC49145-FAE4-4E4E-ACE7-0BAF09922CFD}" name="Pago" dataDxfId="9" totalsRowDxfId="8" dataCellStyle="Moeda" totalsRowCellStyle="Moeda"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1257,22 +1294,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABF31C7A-3C11-4FD7-89F7-C06C471AA575}">
-  <dimension ref="B2:M33"/>
+  <dimension ref="B2:N33"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="24.6640625" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5546875" customWidth="1"/>
-    <col min="6" max="10" width="23.109375" customWidth="1"/>
+    <col min="2" max="2" width="24.6328125" customWidth="1"/>
+    <col min="3" max="3" width="22.08984375" customWidth="1"/>
+    <col min="4" max="4" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.6328125" customWidth="1"/>
+    <col min="6" max="6" width="18.54296875" customWidth="1"/>
+    <col min="7" max="11" width="23.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1283,25 +1321,28 @@
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="H2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -1311,15 +1352,15 @@
       <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
+      <c r="E3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
         <v>9700</v>
       </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
       <c r="H3" s="1">
         <v>0</v>
       </c>
@@ -1327,14 +1368,17 @@
         <v>0</v>
       </c>
       <c r="J3" s="1">
-        <f>SUM(E3:I3)</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <f>SUM(F3:J3)</f>
         <v>9700</v>
       </c>
-      <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
@@ -1344,12 +1388,9 @@
       <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="4">
+      <c r="F4" s="4">
         <v>12640</v>
       </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
       <c r="G4" s="1">
         <v>0</v>
       </c>
@@ -1360,14 +1401,17 @@
         <v>0</v>
       </c>
       <c r="J4" s="1">
-        <f>SUM(E4:I4)</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <f>SUM(F4:J4)</f>
         <v>12640</v>
       </c>
-      <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="N4" s="1"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -1375,32 +1419,35 @@
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="4">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="4">
         <v>3800</v>
       </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
       <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
         <v>5000</v>
       </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
       <c r="I5" s="1">
         <v>0</v>
       </c>
       <c r="J5" s="1">
-        <f t="shared" ref="J5:J17" si="0">SUM(E5:I5)</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" ref="K5:K17" si="0">SUM(F5:J5)</f>
         <v>8800</v>
       </c>
-      <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -1410,30 +1457,33 @@
       <c r="D6" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="4">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1">
+      <c r="E6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" s="4">
         <v>0</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
       </c>
       <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
         <v>3000</v>
       </c>
-      <c r="I6" s="1">
-        <v>0</v>
-      </c>
       <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
         <f t="shared" si="0"/>
         <v>3000</v>
       </c>
-      <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="N6" s="1"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -1441,14 +1491,14 @@
         <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E7" s="4">
+        <v>52</v>
+      </c>
+      <c r="E7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="4">
         <v>1900</v>
       </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
       <c r="G7" s="1">
         <v>0</v>
       </c>
@@ -1459,14 +1509,17 @@
         <v>0</v>
       </c>
       <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
         <f t="shared" si="0"/>
         <v>1900</v>
       </c>
-      <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>15</v>
       </c>
@@ -1474,14 +1527,14 @@
         <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" s="4">
+        <v>51</v>
+      </c>
+      <c r="E8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F8" s="4">
         <v>5800</v>
       </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
       <c r="G8" s="1">
         <v>0</v>
       </c>
@@ -1492,29 +1545,29 @@
         <v>0</v>
       </c>
       <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
         <f t="shared" si="0"/>
         <v>5800</v>
       </c>
-      <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="N8" s="1"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="4">
+        <v>53</v>
+      </c>
+      <c r="F9" s="4">
         <v>453.46</v>
       </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
       <c r="G9" s="1">
         <v>0</v>
       </c>
@@ -1525,29 +1578,29 @@
         <v>0</v>
       </c>
       <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
         <f t="shared" si="0"/>
         <v>453.46</v>
       </c>
-      <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="N9" s="1"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="4">
+        <v>54</v>
+      </c>
+      <c r="F10" s="4">
         <v>274</v>
       </c>
-      <c r="F10" s="1">
-        <v>0</v>
-      </c>
       <c r="G10" s="1">
         <v>0</v>
       </c>
@@ -1558,29 +1611,29 @@
         <v>0</v>
       </c>
       <c r="J10" s="1">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
         <f t="shared" si="0"/>
         <v>274</v>
       </c>
-      <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="N10" s="1"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
         <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
-      </c>
-      <c r="E11" s="4">
+        <v>56</v>
+      </c>
+      <c r="F11" s="4">
         <v>30</v>
       </c>
-      <c r="F11" s="1">
-        <v>0</v>
-      </c>
       <c r="G11" s="1">
         <v>0</v>
       </c>
@@ -1591,29 +1644,32 @@
         <v>0</v>
       </c>
       <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C12" t="s">
         <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" s="4">
+        <v>71</v>
+      </c>
+      <c r="E12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" s="4">
         <v>2350</v>
       </c>
-      <c r="F12" s="1">
-        <v>0</v>
-      </c>
       <c r="G12" s="1">
         <v>0</v>
       </c>
@@ -1624,25 +1680,31 @@
         <v>0</v>
       </c>
       <c r="J12" s="1">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
         <f t="shared" si="0"/>
         <v>2350</v>
       </c>
-      <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="N12" s="1"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="4">
-        <v>2000</v>
-      </c>
-      <c r="F13" s="1">
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" s="4">
+        <v>1800</v>
       </c>
       <c r="G13" s="1">
         <v>0</v>
@@ -1654,26 +1716,26 @@
         <v>0</v>
       </c>
       <c r="J13" s="1">
-        <f>SUM(E13:I13)</f>
-        <v>2000</v>
-      </c>
-      <c r="K13" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="K13" s="1">
+        <f>SUM(F13:J13)</f>
+        <v>1800</v>
+      </c>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="N13" s="1"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="4">
+        <v>22</v>
+      </c>
+      <c r="F14" s="4">
         <v>1000</v>
       </c>
-      <c r="F14" s="1">
-        <v>0</v>
-      </c>
       <c r="G14" s="1">
         <v>0</v>
       </c>
@@ -1684,26 +1746,26 @@
         <v>0</v>
       </c>
       <c r="J14" s="1">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="N14" s="1"/>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>17</v>
       </c>
       <c r="C15" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="4">
+      <c r="F15" s="4">
         <v>1000</v>
       </c>
-      <c r="F15" s="1">
-        <v>0</v>
-      </c>
       <c r="G15" s="1">
         <v>0</v>
       </c>
@@ -1714,26 +1776,26 @@
         <v>0</v>
       </c>
       <c r="J15" s="1">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="N15" s="1"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="4">
+      <c r="F16" s="4">
         <v>5000</v>
       </c>
-      <c r="F16" s="1">
-        <v>0</v>
-      </c>
       <c r="G16" s="1">
         <v>0</v>
       </c>
@@ -1744,26 +1806,26 @@
         <v>0</v>
       </c>
       <c r="J16" s="1">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1">
         <f t="shared" si="0"/>
         <v>5000</v>
       </c>
-      <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="N16" s="1"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>18</v>
       </c>
       <c r="C17" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="4">
+      <c r="F17" s="4">
         <v>20000</v>
       </c>
-      <c r="F17" s="1">
-        <v>0</v>
-      </c>
       <c r="G17" s="1">
         <v>0</v>
       </c>
@@ -1774,44 +1836,46 @@
         <v>0</v>
       </c>
       <c r="J17" s="1">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1">
         <f t="shared" si="0"/>
         <v>20000</v>
       </c>
-      <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E18" s="1">
-        <f t="shared" ref="E18:J18" si="1">SUM(E3:E17)</f>
-        <v>56247.46</v>
-      </c>
+      <c r="N17" s="1"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.35">
       <c r="F18" s="1">
+        <f t="shared" ref="F18:K18" si="1">SUM(F3:F17)</f>
+        <v>56047.46</v>
+      </c>
+      <c r="G18" s="1">
         <f t="shared" si="1"/>
         <v>9700</v>
       </c>
-      <c r="G18" s="1">
+      <c r="H18" s="1">
         <f t="shared" si="1"/>
         <v>5000</v>
       </c>
-      <c r="H18" s="1">
+      <c r="I18" s="1">
         <f t="shared" si="1"/>
         <v>3000</v>
       </c>
-      <c r="I18" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="J18" s="1">
         <f t="shared" si="1"/>
-        <v>73947.459999999992</v>
-      </c>
-      <c r="K18" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
+        <f t="shared" si="1"/>
+        <v>73747.459999999992</v>
+      </c>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E19" s="1"/>
+      <c r="N18" s="1"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.35">
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -1820,9 +1884,9 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E20" s="1"/>
+      <c r="N19" s="1"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.35">
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -1831,9 +1895,9 @@
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E21" s="1"/>
+      <c r="N20" s="1"/>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.35">
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -1842,9 +1906,9 @@
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E22" s="1"/>
+      <c r="N21" s="1"/>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.35">
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -1853,9 +1917,9 @@
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E23" s="1"/>
+      <c r="N22" s="1"/>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.35">
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -1864,9 +1928,9 @@
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E24" s="1"/>
+      <c r="N23" s="1"/>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.35">
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -1875,9 +1939,9 @@
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E25" s="1"/>
+      <c r="N24" s="1"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.35">
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -1886,9 +1950,9 @@
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E26" s="1"/>
+      <c r="N25" s="1"/>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.35">
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -1897,9 +1961,9 @@
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E27" s="1"/>
+      <c r="N26" s="1"/>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.35">
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -1908,9 +1972,9 @@
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E28" s="1"/>
+      <c r="N27" s="1"/>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.35">
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -1919,9 +1983,9 @@
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E29" s="1"/>
+      <c r="N28" s="1"/>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.35">
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -1930,9 +1994,9 @@
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E30" s="1"/>
+      <c r="N29" s="1"/>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.35">
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -1941,9 +2005,9 @@
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E31" s="1"/>
+      <c r="N30" s="1"/>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.35">
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
@@ -1952,9 +2016,9 @@
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="E32" s="1"/>
+      <c r="N31" s="1"/>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.35">
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -1963,9 +2027,9 @@
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
-    </row>
-    <row r="33" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E33" s="1"/>
+      <c r="N32" s="1"/>
+    </row>
+    <row r="33" spans="6:14" x14ac:dyDescent="0.35">
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -1974,34 +2038,35 @@
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D18">
+  <conditionalFormatting sqref="D2:E18">
     <cfRule type="containsText" priority="9" operator="containsText" text="Em Aberto">
       <formula>NOT(ISERROR(SEARCH("Em Aberto",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C18">
-    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="Pesquisando">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Pesquisando">
       <formula>NOT(ISERROR(SEARCH("Pesquisando",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="Em Aberto">
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Em Aberto">
       <formula>NOT(ISERROR(SEARCH("Em Aberto",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Decidido">
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="Decidido">
       <formula>NOT(ISERROR(SEARCH("Decidido",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Fechado">
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="Fechado">
       <formula>NOT(ISERROR(SEARCH("Fechado",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:F3 F4 H3:J4 E5:J18">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+  <conditionalFormatting sqref="F3:G3 G4 I3:K4 F5:K18">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G4">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+  <conditionalFormatting sqref="H3:H4">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2015,361 +2080,404 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E62BAD73-713F-4798-BECD-62F5407EB50B}">
-  <dimension ref="B2:E31"/>
+  <dimension ref="B2:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="34.109375" customWidth="1"/>
+    <col min="2" max="2" width="34.08984375" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.453125" customWidth="1"/>
+    <col min="5" max="5" width="16.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B2" s="30" t="s">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B2" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B3" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B4" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="29" t="s">
+      <c r="C4" s="20">
+        <v>43890</v>
+      </c>
+      <c r="D4" s="21"/>
+      <c r="E4" s="22">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B5" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="20">
+        <v>43951</v>
+      </c>
+      <c r="D5" s="21"/>
+      <c r="E5" s="22">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B6" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="28">
+        <v>43963</v>
+      </c>
+      <c r="D6" s="29"/>
+      <c r="E6" s="30">
+        <v>1760</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B7" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="20">
+        <v>43987</v>
+      </c>
+      <c r="D7" s="21"/>
+      <c r="E7" s="22">
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B8" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="20">
+        <v>44005</v>
+      </c>
+      <c r="D8" s="21"/>
+      <c r="E8" s="24">
+        <v>757.43</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B9" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="20">
+        <v>44012</v>
+      </c>
+      <c r="D9" s="21"/>
+      <c r="E9" s="22">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B10" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="20">
+        <v>44012</v>
+      </c>
+      <c r="D10" s="21"/>
+      <c r="E10" s="24">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B11" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="20">
+        <v>44013</v>
+      </c>
+      <c r="D11" s="21"/>
+      <c r="E11" s="22">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B12" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="28">
+        <v>44021</v>
+      </c>
+      <c r="D12" s="29"/>
+      <c r="E12" s="30">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B13" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="28">
+        <v>44042</v>
+      </c>
+      <c r="D13" s="31"/>
+      <c r="E13" s="30">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B14" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="28">
+        <v>44073</v>
+      </c>
+      <c r="D14" s="29"/>
+      <c r="E14" s="33">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B15" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="28">
+        <v>44073</v>
+      </c>
+      <c r="D15" s="29"/>
+      <c r="E15" s="30">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B16" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="28">
+        <v>44073</v>
+      </c>
+      <c r="D16" s="29"/>
+      <c r="E16" s="33">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B17" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="28">
+        <v>44073</v>
+      </c>
+      <c r="D17" s="31"/>
+      <c r="E17" s="30">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B18" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="28">
+        <v>44104</v>
+      </c>
+      <c r="D18" s="29"/>
+      <c r="E18" s="30">
+        <v>182.56</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B19" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="28">
+        <v>44124</v>
+      </c>
+      <c r="D19" s="29"/>
+      <c r="E19" s="30">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B20" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="28">
+        <v>44163</v>
+      </c>
+      <c r="D20" s="29"/>
+      <c r="E20" s="30">
+        <v>75.37</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B21" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="28">
+        <v>44163</v>
+      </c>
+      <c r="D21" s="29"/>
+      <c r="E21" s="30">
+        <v>319.95</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B22" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="28">
+        <v>44163</v>
+      </c>
+      <c r="D22" s="29"/>
+      <c r="E22" s="30">
+        <v>199.9</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B23" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="28">
+        <v>44178</v>
+      </c>
+      <c r="D23" s="29"/>
+      <c r="E23" s="30">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B24" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D24" s="17">
+        <v>4640</v>
+      </c>
+      <c r="E24" s="17"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B25" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="17">
+        <f>8800-E6</f>
+        <v>7040</v>
+      </c>
+      <c r="E25" s="17"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B26" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="17">
+        <v>900</v>
+      </c>
+      <c r="E26" s="17"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B27" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="17">
+        <v>760</v>
+      </c>
+      <c r="E27" s="17"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B28" s="7"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="13">
+        <f>SUM(D4:D27)</f>
+        <v>13340</v>
+      </c>
+      <c r="E28" s="14">
+        <f>SUM(E4:E27)</f>
+        <v>20502.210000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B31" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B32" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="29" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="24">
-        <v>43890</v>
-      </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="26">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="24">
-        <v>43951</v>
-      </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="26">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="24">
-        <v>43987</v>
-      </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="26">
-        <v>2900</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B7" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="24">
-        <v>44005</v>
-      </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="28">
-        <v>757.43</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B8" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="24">
-        <v>44012</v>
-      </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="26">
-        <v>1140</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B9" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="24">
-        <v>44012</v>
-      </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="28">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B10" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="24">
-        <v>44013</v>
-      </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="26">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B11" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" s="16">
-        <v>44021</v>
-      </c>
-      <c r="D11" s="17">
-        <v>1115</v>
-      </c>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B12" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="16">
-        <v>44042</v>
-      </c>
-      <c r="D12" s="17">
-        <v>580</v>
-      </c>
-      <c r="E12" s="17"/>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="16">
-        <v>44073</v>
-      </c>
-      <c r="D13" s="17">
-        <v>1000</v>
-      </c>
-      <c r="E13" s="17"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="16">
-        <v>44073</v>
-      </c>
-      <c r="D14" s="18">
-        <v>580</v>
-      </c>
-      <c r="E14" s="17"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B15" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="16">
-        <v>44073</v>
-      </c>
-      <c r="D15" s="17">
-        <v>2000</v>
-      </c>
-      <c r="E15" s="20"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" s="16">
-        <v>44104</v>
-      </c>
-      <c r="D16" s="18">
-        <v>580</v>
-      </c>
-      <c r="E16" s="17"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="16">
-        <v>44134</v>
-      </c>
-      <c r="D17" s="17">
-        <v>580</v>
-      </c>
-      <c r="E17" s="17"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="16" t="s">
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B33" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="17">
-        <v>4640</v>
-      </c>
-      <c r="E18" s="17"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="17">
-        <v>3800</v>
-      </c>
-      <c r="E19" s="17"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="17">
-        <v>1000</v>
-      </c>
-      <c r="E20" s="17"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="17">
-        <v>760</v>
-      </c>
-      <c r="E21" s="17"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="22">
-        <v>1000</v>
-      </c>
-      <c r="E22" s="17"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B23" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="22">
-        <v>1000</v>
-      </c>
-      <c r="E23" s="17"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="7"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="13">
-        <f>SUM(D4:D23)</f>
-        <v>18635</v>
-      </c>
-      <c r="E24" s="14">
-        <f>SUM(E4:E23)</f>
-        <v>11377.43</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B27" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B28" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="D28" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="E28" s="29" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B29" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="11">
+      <c r="C33" s="5"/>
+      <c r="D33" s="11">
         <v>5000</v>
       </c>
-      <c r="E29" s="6"/>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B30" s="10" t="s">
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B34" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="11">
+      <c r="C34" s="5"/>
+      <c r="D34" s="11">
         <v>20000</v>
       </c>
-      <c r="E30" s="6"/>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C31" s="5"/>
-      <c r="D31" s="12">
-        <f>SUM(D29:D30)</f>
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C35" s="5"/>
+      <c r="D35" s="12">
+        <f>SUM(D33:D34)</f>
         <v>25000</v>
       </c>
-      <c r="E31" s="6"/>
+      <c r="E35" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B31:E31"/>
   </mergeCells>
-  <conditionalFormatting sqref="E5:E6 D7 E8 D9:D12 E18:E20 D14:D17 E24 D13:E13 D11:E11">
-    <cfRule type="cellIs" dxfId="3" priority="11" operator="equal">
+  <conditionalFormatting sqref="E5:E7 D8 E9 D10:D11 E12:E28">
+    <cfRule type="cellIs" dxfId="1" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E21:E23">
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D22:D23">
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E30">
+  <conditionalFormatting sqref="E34">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>